<commit_message>
Data updated by GitHub Bot (2020-06-18 12:10) (#142)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3925C0-727D-4AE3-82D9-F83297781159}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -438,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J99" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -452,16 +453,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -734,11 +735,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:J98"/>
+      <selection activeCell="A99" sqref="A99:J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3892,6 +3893,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-21 12:10) (#155)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE09CBD-7DAA-4C74-9BA3-7F1963AA8E06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9006D0F7-09D7-4EC0-A0E3-11905E8C747A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J101" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J102" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J102" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -736,28 +736,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:J101"/>
+      <selection activeCell="A102" sqref="A102:J102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -949,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>43976</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
         <v>43977</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
         <v>43978</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
         <v>43979</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>43980</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
         <v>43981</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
         <v>43982</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
         <v>43983</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
         <v>43984</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>43985</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="26">
         <v>43986</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="29">
         <v>43987</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="23">
         <v>43988</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="29">
         <v>43989</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
         <v>43990</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="20">
         <v>43991</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="23">
         <v>43992</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="29">
         <v>43993</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="23">
         <v>43994</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="29">
         <v>43995</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="23">
         <v>43996</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
         <v>43997</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="20">
         <v>43998</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="29">
         <v>43999</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
         <v>44000</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="29">
         <v>44001</v>
       </c>
@@ -3986,6 +3986,38 @@
         <v>109</v>
       </c>
       <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-24 12:10) (#169)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA752B0-19CD-4160-85F2-84C90D1D3AA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -55,11 +56,14 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -438,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J104" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J105" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J105" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -452,16 +456,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -734,11 +738,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+      <selection activeCell="A105" sqref="A105:J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,6 +4088,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-25 12:10) (#177)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA752B0-19CD-4160-85F2-84C90D1D3AA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5AFACD-32B5-4F54-9BDF-A42BD6F56F00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -442,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J105" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J105" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J106" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -739,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:J105"/>
+      <selection activeCell="A106" sqref="A106:J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4120,6 +4120,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-27 12:09) (#188)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -441,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J107" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J108" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J108">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -738,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4183,6 +4183,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-28 12:10)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -441,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J108" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J109" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J109">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -738,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J108" sqref="J108"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4215,6 +4215,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>